<commit_message>
Fix formatting for printing
</commit_message>
<xml_diff>
--- a/ti-99-matrix.xlsx
+++ b/ti-99-matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hans/Development/xirtam/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38C53BF-FDA1-4749-B206-F4255C3BCB33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2D87A1-76D7-4642-9005-C907004B40A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36660" yWindow="8160" windowWidth="24120" windowHeight="17380" xr2:uid="{6066424F-8399-B141-8EE7-984BDAAE5CDB}"/>
+    <workbookView xWindow="9000" yWindow="1340" windowWidth="24120" windowHeight="17380" xr2:uid="{6066424F-8399-B141-8EE7-984BDAAE5CDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -243,7 +243,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -251,14 +251,125 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -573,10 +684,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C923CD41-9FEB-034F-85F4-ED76EE223D68}">
-  <dimension ref="B2:L11"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -595,303 +709,355 @@
     <col min="13" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="E2" s="2" t="s">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+    </row>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="13" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="E3" s="1">
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="5">
         <v>1</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="3">
         <v>2</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="3">
         <v>3</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="3">
         <v>4</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="3">
         <v>5</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="3">
         <v>7</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="3">
         <v>10</v>
       </c>
-      <c r="L3" s="1">
+      <c r="L3" s="10">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="E4" s="1" t="s">
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" s="10" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B5" s="2" t="s">
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B5" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="7">
         <v>6</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B6" s="2" t="s">
+      <c r="K5" s="3"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="3">
         <v>8</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="3">
         <v>0</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="3">
         <v>1</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="K6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="L6" s="10" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B7" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="3">
         <v>9</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="3">
         <v>6</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="3">
         <v>5</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="L7" s="10" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B8" s="2" t="s">
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B8" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="3">
         <v>12</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="F8" s="3"/>
+      <c r="G8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="K8" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B9" s="2" t="s">
+      <c r="L8" s="10"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B9" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="3">
         <v>13</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="3">
         <v>9</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="3">
         <v>2</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="K9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="L9" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B10" s="2" t="s">
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B10" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="3">
         <v>14</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="3">
         <v>8</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="I10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="3">
         <v>3</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="K10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="L10" s="10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B11" s="2" t="s">
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B11" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="9">
         <v>15</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="9">
         <v>7</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11" s="9">
         <v>4</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="K11" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="L11" s="11" t="s">
         <v>21</v>
       </c>
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>